<commit_message>
Updated Initial Assessment Report
</commit_message>
<xml_diff>
--- a/public/Excel Results/ Administrative Aide III-1.xlsx
+++ b/public/Excel Results/ Administrative Aide III-1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>C O M P A R A T I V E    A S S E S S M E N T   F O R M</t>
   </si>
@@ -106,6 +106,9 @@
     <t>REMARKS</t>
   </si>
   <si>
+    <t>AVISS HUELS</t>
+  </si>
+  <si>
     <t>Position</t>
   </si>
   <si>
@@ -113,6 +116,12 @@
   </si>
   <si>
     <t>Age/Civil Status</t>
+  </si>
+  <si>
+    <t>CASSANDREA CORMIER</t>
+  </si>
+  <si>
+    <t>GERMAINES FRANECKI</t>
   </si>
   <si>
     <r>
@@ -578,6 +587,15 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -591,15 +609,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -631,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -851,6 +860,34 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
@@ -859,30 +896,46 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="15" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="16" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="14" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="15" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="0" borderId="16" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
@@ -919,61 +972,25 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
     <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1338,10 +1355,10 @@
     <tabColor rgb="FF00B050"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C18" sqref="A1:XFD1048576"/>
+      <selection activeCell="C20" sqref="C10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1369,63 +1386,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="73" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1438,11 +1455,11 @@
       <c r="O3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="9"/>
@@ -1451,11 +1468,11 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1468,84 +1485,84 @@
       <c r="O4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
       <c r="L6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="M6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="57"/>
+      <c r="N6" s="65"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
       <c r="L7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="57"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -1573,16 +1590,16 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" customHeight="1" ht="39">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="72"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="11" t="s">
         <v>18</v>
       </c>
@@ -1595,10 +1612,10 @@
       <c r="L9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="70" t="s">
+      <c r="M9" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="72"/>
+      <c r="N9" s="84"/>
       <c r="O9" s="11" t="s">
         <v>23</v>
       </c>
@@ -1623,394 +1640,400 @@
         <v>1</v>
       </c>
       <c r="B10" s="39"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
+      <c r="C10" s="89" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
       <c r="K10" s="40"/>
       <c r="L10" s="54"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="61"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="71"/>
       <c r="O10" s="45"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
       <c r="R10" s="42"/>
       <c r="S10" s="43"/>
-      <c r="T10" s="87"/>
+      <c r="T10" s="63"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="14"/>
       <c r="B11" s="44">
         <f>B10</f>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
+      <c r="C11" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
       <c r="K11" s="18"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="63"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="73"/>
       <c r="O11" s="46"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
-      <c r="T11" s="88"/>
+      <c r="T11" s="64"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="14"/>
       <c r="B12" s="44">
         <f>B10</f>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
+      <c r="C12" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
       <c r="K12" s="18"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="63"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="46"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="76"/>
+      <c r="T12" s="59"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="14"/>
       <c r="B13" s="44">
         <f>B10</f>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
+      <c r="C13" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
       <c r="K13" s="18"/>
       <c r="L13" s="21"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="63"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="73"/>
       <c r="O13" s="46"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
-      <c r="T13" s="76"/>
+      <c r="T13" s="59"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="14"/>
       <c r="B14" s="44"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
       <c r="K14" s="18"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="73"/>
       <c r="O14" s="46"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
-      <c r="T14" s="76"/>
+      <c r="T14" s="59"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="44"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
+      <c r="C15" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
       <c r="K15" s="18"/>
       <c r="L15" s="21"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="63"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="73"/>
       <c r="O15" s="46"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="16"/>
       <c r="S15" s="17"/>
-      <c r="T15" s="76"/>
+      <c r="T15" s="59"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="14"/>
       <c r="B16" s="44"/>
       <c r="C16" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
+        <v>30</v>
+      </c>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
       <c r="K16" s="18"/>
       <c r="L16" s="21"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="63"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="73"/>
       <c r="O16" s="46"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="76"/>
+      <c r="T16" s="59"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="14"/>
       <c r="B17" s="44"/>
       <c r="C17" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
+        <v>31</v>
+      </c>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
       <c r="K17" s="18"/>
       <c r="L17" s="21"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="63"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="73"/>
       <c r="O17" s="46"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="16"/>
       <c r="S17" s="17"/>
-      <c r="T17" s="76"/>
+      <c r="T17" s="59"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="14"/>
       <c r="B18" s="44"/>
       <c r="C18" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
+        <v>32</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
       <c r="K18" s="18"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="63"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="73"/>
       <c r="O18" s="46"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="16"/>
       <c r="S18" s="17"/>
-      <c r="T18" s="76"/>
+      <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="14"/>
       <c r="B19" s="44"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
       <c r="K19" s="18"/>
       <c r="L19" s="21"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="63"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="73"/>
       <c r="O19" s="46"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
       <c r="R19" s="16"/>
       <c r="S19" s="17"/>
-      <c r="T19" s="76"/>
-    </row>
-    <row r="20" spans="1:20" customHeight="1" ht="16.5">
-      <c r="A20" s="53"/>
-      <c r="B20" s="47">
+      <c r="T19" s="59"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="14">
+        <v>3</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="59"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="14"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="59"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="14"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="59"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="14"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="73"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="59"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="14"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="59"/>
+    </row>
+    <row r="25" spans="1:20" customHeight="1" ht="16.5">
+      <c r="A25" s="53"/>
+      <c r="B25" s="47">
         <f>B10</f>
       </c>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="78"/>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="R21" s="21"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="21"/>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="21"/>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="5" t="s">
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="52"/>
+      <c r="T25" s="61"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="21"/>
-    </row>
-    <row r="24" spans="1:20" customHeight="1" ht="16.5">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="21"/>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="5"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="67"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="21"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="5"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="20"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
@@ -2019,228 +2042,220 @@
       <c r="L26" s="10"/>
       <c r="M26" s="20"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" s="21"/>
       <c r="S26" s="1"/>
       <c r="T26" s="21"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="N27" s="25"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
       <c r="S27" s="1"/>
       <c r="T27" s="21"/>
     </row>
-    <row r="28" spans="1:20" customHeight="1" ht="16.5">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:20">
+      <c r="A28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="21"/>
+    </row>
+    <row r="29" spans="1:20" customHeight="1" ht="16.5">
+      <c r="A29" s="5"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="21"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="21"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="21"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8" t="s">
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="N28" s="8"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="21"/>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="8" t="s">
+      <c r="N32" s="25"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="21"/>
+    </row>
+    <row r="33" spans="1:20" customHeight="1" ht="16.5">
+      <c r="A33" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N29" s="8"/>
-      <c r="O29" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="P29" s="67"/>
-      <c r="Q29" s="67"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="21"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N30" s="8"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="21"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="8"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="21"/>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="8"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="21"/>
-    </row>
-    <row r="33" spans="1:20">
-      <c r="A33" s="8"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="I33" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="J33" s="8"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N33" s="8"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
       <c r="S33" s="28"/>
       <c r="T33" s="21"/>
     </row>
     <row r="34" spans="1:20">
-      <c r="A34" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
+      <c r="A34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N34" s="8"/>
+      <c r="O34" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="P34" s="79"/>
+      <c r="Q34" s="79"/>
+      <c r="R34" s="79"/>
       <c r="S34" s="28"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="35" spans="1:20" customHeight="1" ht="18.75">
+    <row r="35" spans="1:20">
       <c r="A35" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2250,56 +2265,50 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N35" s="8"/>
-      <c r="O35" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
       <c r="S35" s="28"/>
       <c r="T35" s="21"/>
     </row>
     <row r="36" spans="1:20">
-      <c r="A36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="8"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="I36" s="8"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N36" s="8"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P36" s="10"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="8"/>
       <c r="S36" s="28"/>
       <c r="T36" s="21"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="2"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -2307,21 +2316,21 @@
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="8"/>
       <c r="S37" s="28"/>
       <c r="T37" s="21"/>
     </row>
     <row r="38" spans="1:20">
-      <c r="A38" s="31"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -2329,123 +2338,253 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="8"/>
-      <c r="S38" s="1"/>
+      <c r="S38" s="28"/>
       <c r="T38" s="21"/>
     </row>
     <row r="39" spans="1:20">
-      <c r="A39" s="31"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="2"/>
-    </row>
-    <row r="40" spans="1:20">
-      <c r="A40" s="2"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="2"/>
+      <c r="A39" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="21"/>
+    </row>
+    <row r="40" spans="1:20" customHeight="1" ht="18.75">
+      <c r="A40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="21"/>
     </row>
     <row r="41" spans="1:20">
-      <c r="A41" s="2"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="34"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="2"/>
+      <c r="A41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N41" s="8"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="28"/>
+      <c r="T41" s="21"/>
     </row>
     <row r="42" spans="1:20">
-      <c r="A42" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="21"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="2"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="21"/>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="A43" s="31"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="21"/>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="A44" s="31"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="2"/>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" s="2"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="2"/>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="A46" s="2"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="2"/>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="33"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="2"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F25:H25"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="A1:R2"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O25:R25"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O30:R30"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="M32:N32"/>
     <mergeCell ref="G3:K4"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="O3:T3"/>
@@ -2455,30 +2594,30 @@
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="F6:K6"/>
     <mergeCell ref="F7:K7"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O39:R39"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:L33"/>
+    <mergeCell ref="M33:N33"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="I34:L34"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="O34:R34"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:R29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O31:P31"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="I35:L35"/>
     <mergeCell ref="M35:N35"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:R40"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="M41:N41"/>
     <mergeCell ref="O4:T4"/>
-    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="M10:N10"/>
@@ -2491,18 +2630,48 @@
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="M24:N24"/>
   </mergeCells>
-  <conditionalFormatting sqref="O34:R34">
+  <conditionalFormatting sqref="O39:R39">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R10:R20">
+  <conditionalFormatting sqref="R10:R25">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10:T20 A9:T9 A21:Q21 S21:T21 A22:T27 A28:H28 M28:T28 A29:T33 A35:N41 O35:T258 B42:N42 A43:N258 I10:M20 A10:C20 F13:F20">
+  <conditionalFormatting sqref="O10:T25 A9:T9 A10:C25 I10:M25 F13:F25 A26:Q26 S26:T26 A27:T32 A33:H33 M33:T33 A34:T38 A40:N46 O40:T263 B47:N47 A48:N263">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$T9="ABSENT"</formula>
     </cfRule>
@@ -2550,61 +2719,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="7" t="s">
         <v>3</v>
       </c>
@@ -2614,12 +2783,12 @@
       <c r="N3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="9"/>
@@ -2628,11 +2797,11 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2640,77 +2809,77 @@
       <c r="N4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
       <c r="L6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
       <c r="L7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -2738,16 +2907,16 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" customHeight="1" ht="39">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="72"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="11" t="s">
         <v>18</v>
       </c>
@@ -2760,10 +2929,10 @@
       <c r="L9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="70" t="s">
+      <c r="M9" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="72"/>
+      <c r="N9" s="84"/>
       <c r="O9" s="11" t="s">
         <v>23</v>
       </c>
@@ -2788,152 +2957,152 @@
         <v>1</v>
       </c>
       <c r="B10" s="39"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
       <c r="K10" s="40"/>
       <c r="L10" s="54"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="61"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="71"/>
       <c r="O10" s="45"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
       <c r="R10" s="42"/>
       <c r="S10" s="43"/>
-      <c r="T10" s="87"/>
+      <c r="T10" s="63"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="14"/>
       <c r="B11" s="44">
         <f>B10</f>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
+      <c r="C11" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
       <c r="K11" s="18"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="63"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="73"/>
       <c r="O11" s="46"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
-      <c r="T11" s="88"/>
+      <c r="T11" s="64"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="14"/>
       <c r="B12" s="44">
         <f>B10</f>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
+      <c r="C12" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
       <c r="K12" s="18"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="63"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="46"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="76"/>
+      <c r="T12" s="59"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="14"/>
       <c r="B13" s="44">
         <f>B10</f>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
+      <c r="C13" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
       <c r="K13" s="18"/>
       <c r="L13" s="21"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="63"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="73"/>
       <c r="O13" s="46"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
-      <c r="T13" s="76"/>
+      <c r="T13" s="59"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="14"/>
       <c r="B14" s="44"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
       <c r="K14" s="18"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="73"/>
       <c r="O14" s="46"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
-      <c r="T14" s="76"/>
+      <c r="T14" s="59"/>
     </row>
     <row r="15" spans="1:20" customHeight="1" ht="16.5">
       <c r="A15" s="53"/>
       <c r="B15" s="47">
         <f>B10</f>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
       <c r="K15" s="48"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="59"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="67"/>
       <c r="O15" s="49"/>
       <c r="P15" s="50"/>
       <c r="Q15" s="50"/>
       <c r="R15" s="51"/>
       <c r="S15" s="52"/>
-      <c r="T15" s="78"/>
+      <c r="T15" s="61"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -2951,13 +3120,13 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T16" s="21"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -2980,7 +3149,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -3037,12 +3206,12 @@
       <c r="L20" s="10"/>
       <c r="M20" s="20"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="67"/>
-      <c r="R20" s="67"/>
+      <c r="O20" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
       <c r="T20" s="21"/>
     </row>
     <row r="21" spans="1:20">
@@ -3065,26 +3234,26 @@
       <c r="T21" s="21"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="66"/>
+      <c r="A22" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="78"/>
       <c r="O22" s="26"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
@@ -3092,26 +3261,26 @@
       <c r="T22" s="21"/>
     </row>
     <row r="23" spans="1:20" customHeight="1" ht="16.5">
-      <c r="A23" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="N23" s="65"/>
+      <c r="A23" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="77"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
       <c r="Q23" s="27"/>
@@ -3120,56 +3289,56 @@
       <c r="T23" s="21"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="N24" s="65"/>
-      <c r="O24" s="67" t="s">
+      <c r="A24" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="N24" s="77"/>
+      <c r="O24" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
       <c r="S24" s="28"/>
       <c r="T24" s="21"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="N25" s="65"/>
+      <c r="A25" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="77"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="77"/>
       <c r="O25" s="26"/>
       <c r="P25" s="25"/>
       <c r="Q25" s="25"/>
@@ -3192,10 +3361,10 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="P26" s="68"/>
+      <c r="O26" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="P26" s="80"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="8"/>
       <c r="S26" s="28"/>
@@ -3246,86 +3415,86 @@
       <c r="T28" s="21"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="66"/>
-      <c r="O29" s="66" t="s">
+      <c r="A29" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="66"/>
-      <c r="Q29" s="66"/>
-      <c r="R29" s="66"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="78"/>
+      <c r="O29" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="78"/>
       <c r="S29" s="28"/>
       <c r="T29" s="21"/>
     </row>
     <row r="30" spans="1:20" customHeight="1" ht="18.75">
-      <c r="A30" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="N30" s="65"/>
-      <c r="O30" s="65" t="s">
+      <c r="A30" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="65"/>
-      <c r="R30" s="65"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="77"/>
       <c r="S30" s="28"/>
       <c r="T30" s="21"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="N31" s="65"/>
+      <c r="A31" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="N31" s="77"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -3397,7 +3566,7 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3407,6 +3576,7 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="F15:H15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="I31:L31"/>
     <mergeCell ref="M31:N31"/>
@@ -3434,7 +3604,6 @@
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="I23:L23"/>
     <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M15:N15"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="C10:H10"/>
@@ -3467,7 +3636,7 @@
       <formula>#REF!="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10:T15 A9:T9 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253 I10:M15 A10:C15 F13:F15">
+  <conditionalFormatting sqref="O10:T15 A9:T9 A10:C15 I10:M15 F13:F15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$T9="ABSENT"</formula>
     </cfRule>
@@ -3492,7 +3661,7 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3520,61 +3689,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="7" t="s">
         <v>3</v>
       </c>
@@ -3584,12 +3753,12 @@
       <c r="N3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="9"/>
@@ -3598,11 +3767,11 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
@@ -3610,77 +3779,77 @@
       <c r="N4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
       <c r="L6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
       <c r="L7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -3708,16 +3877,16 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" customHeight="1" ht="39">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="72"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="11" t="s">
         <v>18</v>
       </c>
@@ -3730,10 +3899,10 @@
       <c r="L9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="70" t="s">
+      <c r="M9" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="72"/>
+      <c r="N9" s="84"/>
       <c r="O9" s="11" t="s">
         <v>23</v>
       </c>
@@ -3758,152 +3927,152 @@
         <v>1</v>
       </c>
       <c r="B10" s="39"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
       <c r="K10" s="40"/>
       <c r="L10" s="54"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="61"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="71"/>
       <c r="O10" s="45"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
       <c r="R10" s="42"/>
       <c r="S10" s="43"/>
-      <c r="T10" s="87"/>
+      <c r="T10" s="63"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="14"/>
       <c r="B11" s="44">
         <f>B10</f>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
+      <c r="C11" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
       <c r="K11" s="18"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="63"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="73"/>
       <c r="O11" s="46"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
-      <c r="T11" s="88"/>
+      <c r="T11" s="64"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="14"/>
       <c r="B12" s="44">
         <f>B10</f>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
+      <c r="C12" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
       <c r="K12" s="18"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="63"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="46"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="76"/>
+      <c r="T12" s="59"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="14"/>
       <c r="B13" s="44">
         <f>B10</f>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
+      <c r="C13" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
       <c r="K13" s="18"/>
       <c r="L13" s="21"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="63"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="73"/>
       <c r="O13" s="46"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
-      <c r="T13" s="76"/>
+      <c r="T13" s="59"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="14"/>
       <c r="B14" s="44"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
       <c r="K14" s="18"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="73"/>
       <c r="O14" s="46"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
-      <c r="T14" s="76"/>
+      <c r="T14" s="59"/>
     </row>
     <row r="15" spans="1:20" customHeight="1" ht="16.5">
       <c r="A15" s="53"/>
       <c r="B15" s="47">
         <f>B10</f>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
       <c r="K15" s="48"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="59"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="67"/>
       <c r="O15" s="49"/>
       <c r="P15" s="50"/>
       <c r="Q15" s="50"/>
       <c r="R15" s="51"/>
       <c r="S15" s="52"/>
-      <c r="T15" s="78"/>
+      <c r="T15" s="61"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -3921,13 +4090,13 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T16" s="21"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -3950,7 +4119,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -4007,12 +4176,12 @@
       <c r="L20" s="10"/>
       <c r="M20" s="20"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="67"/>
-      <c r="R20" s="67"/>
+      <c r="O20" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
       <c r="T20" s="21"/>
     </row>
     <row r="21" spans="1:20">
@@ -4035,26 +4204,26 @@
       <c r="T21" s="21"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="66"/>
+      <c r="A22" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="78"/>
       <c r="O22" s="26"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
@@ -4062,26 +4231,26 @@
       <c r="T22" s="21"/>
     </row>
     <row r="23" spans="1:20" customHeight="1" ht="16.5">
-      <c r="A23" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="N23" s="65"/>
+      <c r="A23" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="77"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
       <c r="Q23" s="27"/>
@@ -4090,56 +4259,56 @@
       <c r="T23" s="21"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="N24" s="65"/>
-      <c r="O24" s="67" t="s">
+      <c r="A24" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="N24" s="77"/>
+      <c r="O24" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
       <c r="S24" s="28"/>
       <c r="T24" s="21"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="N25" s="65"/>
+      <c r="A25" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="77"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="77"/>
       <c r="O25" s="26"/>
       <c r="P25" s="25"/>
       <c r="Q25" s="25"/>
@@ -4162,10 +4331,10 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="P26" s="68"/>
+      <c r="O26" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="P26" s="80"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="8"/>
       <c r="S26" s="28"/>
@@ -4216,86 +4385,86 @@
       <c r="T28" s="21"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="66"/>
-      <c r="O29" s="66" t="s">
+      <c r="A29" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="66"/>
-      <c r="Q29" s="66"/>
-      <c r="R29" s="66"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="78"/>
+      <c r="O29" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="78"/>
       <c r="S29" s="28"/>
       <c r="T29" s="21"/>
     </row>
     <row r="30" spans="1:20" customHeight="1" ht="18.75">
-      <c r="A30" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="N30" s="65"/>
-      <c r="O30" s="65" t="s">
+      <c r="A30" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="65"/>
-      <c r="R30" s="65"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="77"/>
       <c r="S30" s="28"/>
       <c r="T30" s="21"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="N31" s="65"/>
+      <c r="A31" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="N31" s="77"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -4367,7 +4536,7 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -4377,6 +4546,7 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="F15:H15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="I31:L31"/>
     <mergeCell ref="M31:N31"/>
@@ -4404,7 +4574,6 @@
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="I23:L23"/>
     <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M15:N15"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="C10:H10"/>
@@ -4437,7 +4606,7 @@
       <formula>#REF!="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10:T15 A9:T9 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253 I10:M15 A10:C15 F13:F15">
+  <conditionalFormatting sqref="O10:T15 A9:T9 A10:C15 I10:M15 F13:F15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$T9="ABSENT"</formula>
     </cfRule>

</xml_diff>